<commit_message>
improved LD for ESTA demo
</commit_message>
<xml_diff>
--- a/data/source/harbour-info.xlsx
+++ b/data/source/harbour-info.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardz/git/esta/data/source/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA01EB6-9909-CC41-A6D0-F78F3A9298DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - harbour-info" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - harbour-info" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
-  <si>
-    <t>harbour-info</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
   <si>
     <t>location</t>
   </si>
@@ -55,17 +61,6 @@
     <t>88.354403 22.564199</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://en.wikipedia.org/wiki/Arakan#/media/File:Vista_de_Mrauk-U,_ou_Arrakan_(cidade_de_Arracão)_no_primeiro_plano_o_bairro_português.jpg</t>
-    </r>
-  </si>
-  <si>
     <t>Batavia</t>
   </si>
   <si>
@@ -75,17 +70,6 @@
     <t>106.816667 -6.2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://en.wikipedia.org/wiki/Batavia,_Dutch_East_Indies#/media/File:Iacatra_year_1605-1608_drawn1675-1725.jpg</t>
-    </r>
-  </si>
-  <si>
     <t>Bombay</t>
   </si>
   <si>
@@ -104,17 +88,6 @@
     <t>55.5325 -21.114444</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://en.wikipedia.org/wiki/Réunion#/media/File:MaheDeLaBourdonnais_2.JPG</t>
-    </r>
-  </si>
-  <si>
     <t>Cape of Good Hope</t>
   </si>
   <si>
@@ -139,17 +112,6 @@
     <t>79.83 10.77</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://en.wikipedia.org/wiki/Nagapattinam#/media/File:Negapatnam_van_Choromandel.jpg</t>
-    </r>
-  </si>
-  <si>
     <t>England</t>
   </si>
   <si>
@@ -174,17 +136,6 @@
     <t>79.75 11.75</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://en.wikipedia.org/wiki/Fort_St._David#/media/File:Ft_St_David,_c.1763.jpg</t>
-    </r>
-  </si>
-  <si>
     <t>Foulpointe</t>
   </si>
   <si>
@@ -288,51 +239,124 @@
   </si>
   <si>
     <t>49.905641 -16.881392</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/5/51/AMH-7669-NA_Map_of_the_bay_of_Luanda.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/e/e2/AMH-7277-KB_The_river_of_Maningaar_on_Madagascar.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/f/f4/Arracan_%28Arakan%29_Pagoda-Mandalay_%28NYPL_Hades-2359593-4044357%29.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/4/45/Batavia_-_Townhall_1770.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/0/0f/Bombay-fort-1703.JPG</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/9/9c/Rosemont_-_La_culture_du_café_à_l%27île_Bourbon.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/b/b5/Bezetting_van_Kaap_de_Goede_Hoop_met_Franse_hulp%2C_1781_De_Kaap_de_Goede_Hoop_met_Fransehe_hulptroepen_bezet_in_t%27Jaar_1781_%28titel_op_object%29%2C_RP-P-OB-75.370.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/2/2a/Galle_Fort_Between_1640_-_1667.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/6/61/Coromandel_Coast_1753.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/2/2d/London_customs_house_18th_century.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/e/e4/Fort-Dauphin_Flacourt_1650.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/2/2e/Fort_St_David_map_1758.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/1/18/Manda_Fort_Caserne_Foulpointe_Madagascar.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/4/45/Cacault-Bordeaux-1756.JPG</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/8/84/Manuel_Godinho_de_Erédia_-_Description_of_Malacca%2C_Meridional_India_and_Cathay_-_A_Famosa.png</t>
+  </si>
+  <si>
+    <t>Mitsinjo</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/4/42/Mitsinjo_community_association_headquarters_%2815904901931%29.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/2/2b/Celestine-d06-182a.jpg</t>
+  </si>
+  <si>
+    <t>Masulipatnam</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/c/ca/Gezicht_op_Machilipatnam_%28Masulipatnam%29_Masulipatam_%28titel_op_object%29%2C_RP-P-1908-2308.jpg</t>
+  </si>
+  <si>
+    <t>Manakara Sud</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/8/80/Manakara_river.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/5/5b/Van_Keulen_-_De_Z._O._Haven_van_%27t_Eyland_Mauritius.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/b/b7/P_verreauxi_Grandidier.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/6/6c/The_Capture_of_Port_Louis%2C_Cuba%2C_8_March_1748_RMG_BHC0372.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/a/aa/Pulicat%2C_Aerial_view_of_Pellacata-1682.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/7/76/Saint-Denis.Inselin.1707.Haye-Coq.Gardinou.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/1/12/La_baye_de_Spiritu_Santo%2C_côte_occidentale_de_la_Floride._S._Augustin%2C_capitale_de_la_Floride_orientale._LOC_73694478.jpg</t>
+  </si>
+  <si>
+    <t>Manambato</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/0/0d/Manambato-vue_de_la_RN5a.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/3/3d/Storm_Falls_At_Sainte_Marie_Reunion_Island_%28206783797%29.jpeg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -450,54 +474,60 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -508,26 +538,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -726,7 +815,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -745,7 +834,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="2200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="2200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -775,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -801,7 +890,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -827,7 +916,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -853,7 +942,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -879,7 +968,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -905,7 +994,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -931,7 +1020,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -957,7 +1046,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -983,7 +1072,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -996,9 +1085,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1015,7 +1110,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1034,7 +1129,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1060,7 +1155,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1086,7 +1181,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1112,7 +1207,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1138,7 +1233,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1259,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1190,7 +1285,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1216,7 +1311,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1242,7 +1337,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1268,7 +1363,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1281,9 +1376,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1297,7 +1398,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1316,7 +1417,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1346,7 +1447,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1372,7 +1473,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1398,7 +1499,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1424,7 +1525,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1450,7 +1551,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1476,7 +1577,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1502,7 +1603,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1528,7 +1629,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1554,7 +1655,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1567,599 +1668,635 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K29"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="110.172" style="1" customWidth="1"/>
-    <col min="5" max="11" width="8.35156" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="110.1640625" style="2" customWidth="1"/>
+    <col min="5" max="12" width="8.33203125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="D2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="D3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="9">
+      <c r="B4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s" s="10">
+      <c r="C4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="D4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="9">
+      <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s" s="10">
+      <c r="D5" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="B6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="C6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="9">
+      <c r="D6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s" s="10">
+      <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s" s="11">
+      <c r="C7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="9">
+      <c r="D7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s" s="10">
+      <c r="B8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s" s="11">
+      <c r="D8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s" s="11">
+      <c r="B9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="9">
+      <c r="C9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s" s="11">
+      <c r="D9" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="9">
+      <c r="B10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s" s="10">
+      <c r="C10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s" s="11">
+      <c r="D10" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="9">
+      <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s" s="10">
+      <c r="C11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s" s="11">
+      <c r="D11" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s" s="11">
+      <c r="B12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="9">
+      <c r="C12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="s" s="10">
+      <c r="D12" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s" s="11">
+      <c r="B13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="9">
+      <c r="D13" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s" s="10">
+      <c r="B14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s" s="11">
+      <c r="C14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="9">
+      <c r="D14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s" s="11">
+      <c r="B15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D14" t="s" s="11">
+      <c r="C15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="9">
+      <c r="D15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s" s="10">
+      <c r="B16" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s" s="11">
+      <c r="D16" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="9">
+      <c r="B17" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s" s="10">
+      <c r="D17" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="s" s="11">
+      <c r="B18" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="9">
+      <c r="D18" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s" s="10">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s" s="11">
+      <c r="B19" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="9">
+      <c r="C19" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" t="s" s="11">
+      <c r="D19" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="9">
+      <c r="B20" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" t="s" s="14">
+      <c r="D20" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="9">
+      <c r="B21" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s" s="10">
+      <c r="C21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C20" t="s" s="11">
+      <c r="D21" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="9">
+      <c r="B22" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" t="s" s="14">
+      <c r="D22" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="9">
+      <c r="B24" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B22" t="s" s="10">
+      <c r="D24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C22" t="s" s="11">
+      <c r="B25" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="9">
+      <c r="C25" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B23" t="s" s="10">
-        <v>64</v>
-      </c>
-      <c r="C23" t="s" s="11">
+      <c r="D25" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-    </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="9">
-        <v>62</v>
-      </c>
-      <c r="B24" t="s" s="10">
-        <v>62</v>
-      </c>
-      <c r="C24" t="s" s="11">
-        <v>63</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-    </row>
-    <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="9">
+      <c r="B26" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B25" t="s" s="10">
-        <v>66</v>
-      </c>
-      <c r="C25" t="s" s="11">
+      <c r="C26" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-    </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="9">
+      <c r="D26" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B26" t="s" s="10">
+      <c r="B27" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C26" t="s" s="11">
+      <c r="D27" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-    </row>
-    <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="9">
+      <c r="B28" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B27" t="s" s="10">
+      <c r="C28" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C27" t="s" s="11">
-        <v>73</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-    </row>
-    <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="9">
-        <v>74</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" t="s" s="14">
-        <v>75</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-    </row>
-    <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="9">
-        <v>76</v>
-      </c>
-      <c r="B29" t="s" s="10">
-        <v>77</v>
-      </c>
-      <c r="C29" t="s" s="11">
-        <v>78</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
+      <c r="D28" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" location="" tooltip="" display="https://en.wikipedia.org/wiki/Arakan#/media/File:Vista_de_Mrauk-U,_ou_Arrakan_(cidade_de_Arracão)_no_primeiro_plano_o_bairro_português.jpg"/>
-    <hyperlink ref="D6" r:id="rId2" location="" tooltip="" display="https://en.wikipedia.org/wiki/Batavia,_Dutch_East_Indies#/media/File:Iacatra_year_1605-1608_drawn1675-1725.jpg"/>
-    <hyperlink ref="D8" r:id="rId3" location="" tooltip="" display="https://en.wikipedia.org/wiki/Réunion#/media/File:MaheDeLaBourdonnais_2.JPG"/>
-    <hyperlink ref="D11" r:id="rId4" location="" tooltip="" display="https://en.wikipedia.org/wiki/Nagapattinam#/media/File:Negapatnam_van_Choromandel.jpg"/>
-    <hyperlink ref="D14" r:id="rId5" location="" tooltip="" display="https://en.wikipedia.org/wiki/Fort_St._David#/media/File:Ft_St_David,_c.1763.jpg"/>
-  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>